<commit_message>
Correcciones cap 2 y 4
Se actualizaron idicadores del cap 2 y 4.
</commit_message>
<xml_diff>
--- a/Codigo/Bases/datos_administrativos/Indicadores_de_Género/ECONOMÍA_Y_TRABAJO/4-11_4-12.xlsx
+++ b/Codigo/Bases/datos_administrativos/Indicadores_de_Género/ECONOMÍA_Y_TRABAJO/4-11_4-12.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inegobgt-my.sharepoint.com/personal/unidadgenero_ine_gob_gt/Documents/Documentos/Github/CompendioGenero2023/Codigo/Bases/datos_administrativos/Indicadores_de_Género/ECONOMÍA_Y_TRABAJO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pgalvez\OneDrive - ine.gob.gt\Documentos\GitHub\CompendioGenero2023\Codigo\Bases\datos_administrativos\Indicadores_de_Género\ECONOMÍA_Y_TRABAJO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{E35A8450-3881-46A5-90AF-EEDF09049B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4388E90-B361-47A5-A6C0-53B224E4F0A3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3321CB-3FCE-49D8-A3C2-060CC3C58720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{D20D2A10-7D92-4AB5-9CAB-85D403B93368}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{D20D2A10-7D92-4AB5-9CAB-85D403B93368}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
     <sheet name="2018" sheetId="3" r:id="rId2"/>
     <sheet name="2022" sheetId="4" r:id="rId3"/>
-    <sheet name="sexo" sheetId="5" r:id="rId4"/>
+    <sheet name="creditos" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -528,7 +528,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Millares" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -544,12 +544,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -851,7 +847,7 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
@@ -1347,7 +1343,7 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1424,11 +1420,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FCA3B4A-921E-4CF9-9746-7C7DAF14D7A8}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1505,11 +1501,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC933E11-37B2-495D-A46F-3B8EA693FB25}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>

</xml_diff>